<commit_message>
Creacion de recruitment.feature y libro recruitment
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
+++ b/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Recruitment" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -35,14 +36,75 @@
   </si>
   <si>
     <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRST_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIDDLE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAST_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VACANCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTACT_NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEYWORDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA_OF_APPLICATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSENT_TO_KEEP_DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHORTLIST_NOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">de Jesus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernal Lopez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA LEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w@w.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El mejor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-22-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nota1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nota2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -118,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -133,6 +195,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -214,11 +280,11 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.75"/>
   </cols>
@@ -254,4 +320,118 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>3126148527</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="w@w.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continuacion de logica de reclutamiento
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
+++ b/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nota1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">Nota2</t>
@@ -197,8 +200,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -284,7 +287,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.75"/>
   </cols>
@@ -330,10 +333,10 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.22"/>
@@ -388,38 +391,41 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="3" t="n">
         <v>3126148527</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logica de interaccion con el select
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
+++ b/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
@@ -80,7 +80,7 @@
     <t xml:space="preserve">Bernal Lopez</t>
   </si>
   <si>
-    <t xml:space="preserve">QA LEAD</t>
+    <t xml:space="preserve">Junior Account Assistant</t>
   </si>
   <si>
     <t xml:space="preserve">w@w.com</t>
@@ -287,7 +287,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.75"/>
   </cols>
@@ -333,7 +333,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -342,7 +342,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.31"/>

</xml_diff>

<commit_message>
Interaccion con el calendario
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
+++ b/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">KEYWORDS</t>
   </si>
   <si>
-    <t xml:space="preserve">DATA_OF_APPLICATION</t>
+    <t xml:space="preserve">DATE_OF_APPLICATION</t>
   </si>
   <si>
     <t xml:space="preserve">NOTE</t>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">El mejor</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-22-07</t>
+    <t xml:space="preserve">17-07-2024</t>
   </si>
   <si>
     <t xml:space="preserve">Nota1</t>
@@ -287,7 +287,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.75"/>
   </cols>
@@ -333,7 +333,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Logica de selecion de fecha dos
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
+++ b/src/test/resources/datadriven/DataOrangeHrmLive.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wilder </t>
-  </si>
-  <si>
-    <t xml:space="preserve">de Jesus </t>
   </si>
   <si>
     <t xml:space="preserve">Bernal Lopez</t>
@@ -287,7 +284,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.75"/>
   </cols>
@@ -333,7 +330,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -397,35 +394,33 @@
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>3126148527</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>